<commit_message>
renamed spell color to spell type added key to spell slots & spell beans drew new icons for equipment items preparing for weapon spell slots...
</commit_message>
<xml_diff>
--- a/res/items.xlsx
+++ b/res/items.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14115" windowHeight="7755"/>
+    <workbookView xWindow="240" yWindow="132" windowWidth="14112" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="118">
   <si>
     <t>Item ID</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Sprite Offset (x.f, y.f)</t>
   </si>
   <si>
-    <t>level item bounding box (x, y, w, h)</t>
-  </si>
-  <si>
     <t>Texture Positions for level item (x1, y1, w1, h1, x2, y2, w2, h2, …)</t>
   </si>
   <si>
@@ -97,18 +94,12 @@
     <t>itd_wizardhat</t>
   </si>
   <si>
-    <t>100, 100</t>
-  </si>
-  <si>
     <t>res/assets/equipment/head/spritesheet_head_wizardhat_blue.png</t>
   </si>
   <si>
     <t>it_eq_wizardhatgrey</t>
   </si>
   <si>
-    <t>150, 100</t>
-  </si>
-  <si>
     <t>res/assets/equipment/head/spritesheet_head_wizardhat_grey.png</t>
   </si>
   <si>
@@ -118,9 +109,6 @@
     <t>itd_icestaff</t>
   </si>
   <si>
-    <t>200, 100</t>
-  </si>
-  <si>
     <t>res/assets/equipment/weapon/spritesheet_staff_ice.png</t>
   </si>
   <si>
@@ -130,9 +118,6 @@
     <t>itd_rustysword</t>
   </si>
   <si>
-    <t>250, 100</t>
-  </si>
-  <si>
     <t>res/assets/equipment/weapon/spritesheet_weapon_rustysword.png</t>
   </si>
   <si>
@@ -154,9 +139,6 @@
     <t>0, 100</t>
   </si>
   <si>
-    <t>0, 0, 22, 22</t>
-  </si>
-  <si>
     <t>0, 0, 50, 50</t>
   </si>
   <si>
@@ -169,9 +151,6 @@
     <t>50, 100</t>
   </si>
   <si>
-    <t>0, 0, 30, 5</t>
-  </si>
-  <si>
     <t>200, 0, 50, 50</t>
   </si>
   <si>
@@ -184,9 +163,6 @@
     <t>100, 0</t>
   </si>
   <si>
-    <t>0, 0, 18, 30</t>
-  </si>
-  <si>
     <t>200, 50, 50, 50</t>
   </si>
   <si>
@@ -202,9 +178,6 @@
     <t>0, -30</t>
   </si>
   <si>
-    <t>0, 0, 50, 70</t>
-  </si>
-  <si>
     <t>0, 0, 50, 100</t>
   </si>
   <si>
@@ -217,9 +190,6 @@
     <t>150, 50</t>
   </si>
   <si>
-    <t>0, 0, 30, 30</t>
-  </si>
-  <si>
     <t>100, 50, 50, 50</t>
   </si>
   <si>
@@ -235,9 +205,6 @@
     <t>-10, 0</t>
   </si>
   <si>
-    <t>0, 0, 30, 50</t>
-  </si>
-  <si>
     <t>50, 50, 50, 50</t>
   </si>
   <si>
@@ -253,9 +220,6 @@
     <t>0, -20</t>
   </si>
   <si>
-    <t>0, 0, 50, 30</t>
-  </si>
-  <si>
     <t>150, 0, 50, 50</t>
   </si>
   <si>
@@ -268,9 +232,6 @@
     <t>0, 50</t>
   </si>
   <si>
-    <t>0, 0, 30, 40</t>
-  </si>
-  <si>
     <t>50, 0, 50, 50</t>
   </si>
   <si>
@@ -283,18 +244,12 @@
     <t>100, 50</t>
   </si>
   <si>
-    <t>0, 0, 5, 5</t>
-  </si>
-  <si>
     <t>it_go_threecoins</t>
   </si>
   <si>
     <t>itd_threecoins</t>
   </si>
   <si>
-    <t>0, 0, 25, 25</t>
-  </si>
-  <si>
     <t>150, 50, 50, 50</t>
   </si>
   <si>
@@ -329,6 +284,90 @@
   </si>
   <si>
     <t>-14, -40</t>
+  </si>
+  <si>
+    <t>0, 150</t>
+  </si>
+  <si>
+    <t>50, 150</t>
+  </si>
+  <si>
+    <t>100, 150</t>
+  </si>
+  <si>
+    <t>150, 150</t>
+  </si>
+  <si>
+    <t>200, 150</t>
+  </si>
+  <si>
+    <t>weapon chop cooldown (ms)</t>
+  </si>
+  <si>
+    <t>40, 80</t>
+  </si>
+  <si>
+    <t>weapon chop rectangle (0, 0, w, h)</t>
+  </si>
+  <si>
+    <t>40, 50</t>
+  </si>
+  <si>
+    <t>weapon chop damage</t>
+  </si>
+  <si>
+    <t>level item bounding box (0, 0, w, h)</t>
+  </si>
+  <si>
+    <t>22, 22</t>
+  </si>
+  <si>
+    <t>30, 5</t>
+  </si>
+  <si>
+    <t>18, 30</t>
+  </si>
+  <si>
+    <t>50, 70</t>
+  </si>
+  <si>
+    <t>30, 30</t>
+  </si>
+  <si>
+    <t>30, 50</t>
+  </si>
+  <si>
+    <t>50, 30</t>
+  </si>
+  <si>
+    <t>30, 40</t>
+  </si>
+  <si>
+    <t>5, 5</t>
+  </si>
+  <si>
+    <t>25, 25</t>
+  </si>
+  <si>
+    <t>slot 2</t>
+  </si>
+  <si>
+    <t>slot 3</t>
+  </si>
+  <si>
+    <t>slot 4</t>
+  </si>
+  <si>
+    <t>slot 5</t>
+  </si>
+  <si>
+    <t>slot 1 (the first entry is the type (elemental, twilight, necromancy, divine, illusion) and after this, the 0 and 1 show if there is a modifier for this type (strength, duration, range, speed, damage, count, reflect)</t>
+  </si>
+  <si>
+    <t>1, 0, 0, 0, 1, 0, 1, 0</t>
+  </si>
+  <si>
+    <t>1, 0, 0, 0, 0, 1, 0, 1</t>
   </si>
 </sst>
 </file>
@@ -1151,18 +1190,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y17"/>
+  <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1:Z1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="21" max="21" width="11.42578125" style="1"/>
+    <col min="21" max="21" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1227,30 +1266,54 @@
         <v>20</v>
       </c>
       <c r="V1" t="s">
+        <v>100</v>
+      </c>
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="A2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="E2">
         <v>22</v>
@@ -1265,21 +1328,21 @@
         <v>2</v>
       </c>
       <c r="Y2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:33">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="E3">
         <v>20</v>
@@ -1294,21 +1357,21 @@
         <v>2</v>
       </c>
       <c r="Y3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:33">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="E4">
         <v>120</v>
@@ -1323,21 +1386,36 @@
         <v>30</v>
       </c>
       <c r="Y4" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="Z4">
+        <v>500</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB4">
+        <v>10</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:33">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -1346,21 +1424,30 @@
         <v>5</v>
       </c>
       <c r="Y5" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="Z5">
+        <v>350</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB5">
+        <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:33">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C6">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -1372,21 +1459,21 @@
         <v>5</v>
       </c>
       <c r="Y6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:33">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C7">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -1401,30 +1488,30 @@
         <v>10</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="V7" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="W7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="X7">
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:33">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C8">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -1436,30 +1523,30 @@
         <v>15</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="V8" t="s">
-        <v>51</v>
+        <v>102</v>
       </c>
       <c r="W8" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="X8">
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:33">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -1477,30 +1564,30 @@
         <v>5</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="V9" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="W9" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="X9">
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:33">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -1521,30 +1608,30 @@
         <v>20</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="V10" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="W10" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="X10">
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:33">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C11">
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -1562,30 +1649,30 @@
         <v>15</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="V11" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="W11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="X11">
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:33">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C12">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -1597,111 +1684,111 @@
         <v>10</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="V12" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="W12" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="X12">
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:33">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C13">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="V13" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="W13" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="X13">
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:33">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C14">
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E14">
         <v>15</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="V14" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="W14" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="X14">
         <v>1000</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:33">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="E15">
         <v>20</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="V15" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="W15" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="X15">
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:33">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C16">
         <v>13</v>
@@ -1710,13 +1797,13 @@
         <v>3</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="V16" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="W16" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="X16">
         <v>1000</v>
@@ -1724,10 +1811,10 @@
     </row>
     <row r="17" spans="1:24">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C17">
         <v>13</v>
@@ -1736,13 +1823,13 @@
         <v>1</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="V17" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="W17" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="X17">
         <v>1000</v>

</xml_diff>

<commit_message>
added weapons. weapons determine spell slots and their modifiers weapons determine the attributes of their chop spell (bb, cooldown, dmg) the modifiers and equipped spells can now be SAVED in savefiles and loaded from there. use isa's testsave to load a save with predefined equipped spells in a weapon.
</commit_message>
<xml_diff>
--- a/res/items.xlsx
+++ b/res/items.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="120">
   <si>
     <t>Item ID</t>
   </si>
@@ -368,6 +368,12 @@
   </si>
   <si>
     <t>1, 0, 0, 0, 0, 1, 0, 1</t>
+  </si>
+  <si>
+    <t>4, 1,1,1,1, 1, 0, 1</t>
+  </si>
+  <si>
+    <t>4,1,1,1,1,1,1,1</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1199,7 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1:Z1048576"/>
+      <selection activeCell="AF6" sqref="AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1403,6 +1409,12 @@
       <c r="AD4" t="s">
         <v>117</v>
       </c>
+      <c r="AE4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="5" spans="1:33">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
added anti gravity spell!
</commit_message>
<xml_diff>
--- a/res/items.xlsx
+++ b/res/items.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="122">
   <si>
     <t>Item ID</t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>3,1,1,1,1,1,1,1</t>
+  </si>
+  <si>
+    <t>1,1,1,1,1,1,1,1</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1205,7 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AE6" sqref="AE6"/>
+      <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1453,6 +1456,9 @@
       <c r="AB5">
         <v>5</v>
       </c>
+      <c r="AC5" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="6" spans="1:33">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
added dynamic tile: shiftable block added spell: wind gust
</commit_message>
<xml_diff>
--- a/res/items.xlsx
+++ b/res/items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="132" windowWidth="14112" windowHeight="7752"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14115" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="122">
   <si>
     <t>Item ID</t>
   </si>
@@ -1205,12 +1205,12 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AC9" sqref="AC9"/>
+      <selection activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="21" max="21" width="11.44140625" style="1"/>
+    <col min="21" max="21" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -1457,6 +1457,9 @@
         <v>5</v>
       </c>
       <c r="AC5" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD5" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added leech spell collisions now ignore dynamic tiles that are out of view
</commit_message>
<xml_diff>
--- a/res/items.xlsx
+++ b/res/items.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="122">
   <si>
     <t>Item ID</t>
   </si>
@@ -1205,7 +1205,7 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AD5" sqref="AD5"/>
+      <selection activeCell="AE9" sqref="AE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1462,6 +1462,9 @@
       <c r="AD5" t="s">
         <v>121</v>
       </c>
+      <c r="AE5" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="6" spans="1:33">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
added spell: icy ambush redesigned spell: wind gust refactored spells: the argument "divergenceAngle" in Spell::load is saved in the spellbean.
</commit_message>
<xml_diff>
--- a/res/items.xlsx
+++ b/res/items.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="123">
   <si>
     <t>Item ID</t>
   </si>
@@ -380,6 +380,9 @@
   </si>
   <si>
     <t>1,1,1,1,1,1,1,1</t>
+  </si>
+  <si>
+    <t>2,1,1,1,1,1,1,1</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1208,7 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AE9" sqref="AE9"/>
+      <selection activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1465,6 +1468,9 @@
       <c r="AE5" t="s">
         <v>120</v>
       </c>
+      <c r="AF5" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="6" spans="1:33">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
implemented interface consumables can be consumed with right click GOs can decide whether they want to get input in default view or not windows can be resized button colours can be changed
</commit_message>
<xml_diff>
--- a/res/items.xlsx
+++ b/res/items.xlsx
@@ -1207,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AD16" sqref="AD16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1769,7 +1769,7 @@
         <v>70</v>
       </c>
       <c r="C14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
         <v>71</v>
@@ -1827,7 +1827,7 @@
         <v>77</v>
       </c>
       <c r="C16">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -1853,7 +1853,7 @@
         <v>80</v>
       </c>
       <c r="C17">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17">
         <v>1</v>

</xml_diff>

<commit_message>
weapon spell slots & gem sockets appear in the description window weapon spell slots have a maximal number of sockets and not true/false for each modifier type. This number is between 0 and 3. added missing translations
</commit_message>
<xml_diff>
--- a/res/items.xlsx
+++ b/res/items.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="120">
   <si>
     <t>Item ID</t>
   </si>
@@ -361,28 +361,19 @@
     <t>slot 5</t>
   </si>
   <si>
-    <t>slot 1 (the first entry is the type (elemental, twilight, necromancy, divine, illusion) and after this, the 0 and 1 show if there is a modifier for this type (strength, duration, range, speed, damage, count, reflect)</t>
-  </si>
-  <si>
-    <t>1, 0, 0, 0, 1, 0, 1, 0</t>
-  </si>
-  <si>
-    <t>1, 0, 0, 0, 0, 1, 0, 1</t>
-  </si>
-  <si>
-    <t>4, 1,1,1,1, 1, 0, 1</t>
-  </si>
-  <si>
-    <t>4,1,1,1,1,1,1,1</t>
-  </si>
-  <si>
-    <t>3,1,1,1,1,1,1,1</t>
-  </si>
-  <si>
-    <t>1,1,1,1,1,1,1,1</t>
-  </si>
-  <si>
-    <t>2,1,1,1,1,1,1,1</t>
+    <t>1, 3</t>
+  </si>
+  <si>
+    <t>4, 3</t>
+  </si>
+  <si>
+    <t>3, 3</t>
+  </si>
+  <si>
+    <t>2, 3</t>
+  </si>
+  <si>
+    <t>slot 1 (the first entry is the type (elemental, twilight, necromancy, divine, illusion) and after this, the number shows the maximal modifiers for this slot</t>
   </si>
 </sst>
 </file>
@@ -1207,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1302,7 +1293,7 @@
         <v>99</v>
       </c>
       <c r="AC1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="AD1" t="s">
         <v>111</v>
@@ -1413,19 +1404,19 @@
         <v>10</v>
       </c>
       <c r="AC4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE4" t="s">
         <v>116</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AF4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG4" t="s">
         <v>117</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>118</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -1460,16 +1451,16 @@
         <v>5</v>
       </c>
       <c r="AC5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="AD5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="AE5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="AF5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:33">

</xml_diff>

<commit_message>
level screen works on a copy of character core and writes it only on checkpoint down on original core. fixed small cosmetic defects.
</commit_message>
<xml_diff>
--- a/res/items.xlsx
+++ b/res/items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14115" windowHeight="7755"/>
+    <workbookView xWindow="240" yWindow="132" windowWidth="14112" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="121">
   <si>
     <t>Item ID</t>
   </si>
@@ -277,9 +277,6 @@
     <t>-10, -5</t>
   </si>
   <si>
-    <t>-20, -40</t>
-  </si>
-  <si>
     <t>-5, -25</t>
   </si>
   <si>
@@ -304,76 +301,82 @@
     <t>weapon chop cooldown (ms)</t>
   </si>
   <si>
+    <t>weapon chop rectangle (0, 0, w, h)</t>
+  </si>
+  <si>
+    <t>weapon chop damage</t>
+  </si>
+  <si>
+    <t>level item bounding box (0, 0, w, h)</t>
+  </si>
+  <si>
+    <t>22, 22</t>
+  </si>
+  <si>
+    <t>30, 5</t>
+  </si>
+  <si>
+    <t>18, 30</t>
+  </si>
+  <si>
+    <t>50, 70</t>
+  </si>
+  <si>
+    <t>30, 30</t>
+  </si>
+  <si>
+    <t>30, 50</t>
+  </si>
+  <si>
+    <t>50, 30</t>
+  </si>
+  <si>
+    <t>30, 40</t>
+  </si>
+  <si>
+    <t>5, 5</t>
+  </si>
+  <si>
+    <t>25, 25</t>
+  </si>
+  <si>
+    <t>slot 2</t>
+  </si>
+  <si>
+    <t>slot 3</t>
+  </si>
+  <si>
+    <t>slot 4</t>
+  </si>
+  <si>
+    <t>slot 5</t>
+  </si>
+  <si>
+    <t>1, 3</t>
+  </si>
+  <si>
+    <t>4, 3</t>
+  </si>
+  <si>
+    <t>3, 3</t>
+  </si>
+  <si>
+    <t>2, 3</t>
+  </si>
+  <si>
+    <t>slot 1 (the first entry is the type (elemental, twilight, necromancy, divine, illusion) and after this, the number shows the maximal modifiers for this slot</t>
+  </si>
+  <si>
+    <t>45, 80</t>
+  </si>
+  <si>
     <t>40, 80</t>
   </si>
   <si>
-    <t>weapon chop rectangle (0, 0, w, h)</t>
-  </si>
-  <si>
-    <t>40, 50</t>
-  </si>
-  <si>
-    <t>weapon chop damage</t>
-  </si>
-  <si>
-    <t>level item bounding box (0, 0, w, h)</t>
-  </si>
-  <si>
-    <t>22, 22</t>
-  </si>
-  <si>
-    <t>30, 5</t>
-  </si>
-  <si>
-    <t>18, 30</t>
-  </si>
-  <si>
-    <t>50, 70</t>
-  </si>
-  <si>
-    <t>30, 30</t>
-  </si>
-  <si>
-    <t>30, 50</t>
-  </si>
-  <si>
-    <t>50, 30</t>
-  </si>
-  <si>
-    <t>30, 40</t>
-  </si>
-  <si>
-    <t>5, 5</t>
-  </si>
-  <si>
-    <t>25, 25</t>
-  </si>
-  <si>
-    <t>slot 2</t>
-  </si>
-  <si>
-    <t>slot 3</t>
-  </si>
-  <si>
-    <t>slot 4</t>
-  </si>
-  <si>
-    <t>slot 5</t>
-  </si>
-  <si>
-    <t>1, 3</t>
-  </si>
-  <si>
-    <t>4, 3</t>
-  </si>
-  <si>
-    <t>3, 3</t>
-  </si>
-  <si>
-    <t>2, 3</t>
-  </si>
-  <si>
-    <t>slot 1 (the first entry is the type (elemental, twilight, necromancy, divine, illusion) and after this, the number shows the maximal modifiers for this slot</t>
+    <t>8, 8</t>
+  </si>
+  <si>
+    <t>-18, -34</t>
   </si>
 </sst>
 </file>
@@ -1198,13 +1201,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AG8" sqref="AG8"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="21" max="21" width="11.42578125" style="1"/>
+    <col min="21" max="21" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -1272,7 +1275,7 @@
         <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="W1" t="s">
         <v>21</v>
@@ -1284,28 +1287,28 @@
         <v>23</v>
       </c>
       <c r="Z1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA1" t="s">
         <v>95</v>
       </c>
-      <c r="AA1" t="s">
-        <v>97</v>
-      </c>
       <c r="AB1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AC1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AD1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG1" t="s">
         <v>111</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>112</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>113</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:33">
@@ -1319,7 +1322,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E2">
         <v>22</v>
@@ -1348,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E3">
         <v>20</v>
@@ -1377,7 +1380,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4">
         <v>120</v>
@@ -1398,25 +1401,25 @@
         <v>500</v>
       </c>
       <c r="AA4" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="AB4">
         <v>10</v>
       </c>
       <c r="AC4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="AD4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="AE4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AF4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AG4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:33">
@@ -1430,7 +1433,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -1445,22 +1448,22 @@
         <v>350</v>
       </c>
       <c r="AA5" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="AB5">
         <v>5</v>
       </c>
       <c r="AC5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF5" t="s">
         <v>115</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>115</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>117</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -1474,7 +1477,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -1518,7 +1521,7 @@
         <v>82</v>
       </c>
       <c r="V7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="W7" t="s">
         <v>41</v>
@@ -1553,7 +1556,7 @@
         <v>83</v>
       </c>
       <c r="V8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="W8" t="s">
         <v>45</v>
@@ -1594,7 +1597,7 @@
         <v>84</v>
       </c>
       <c r="V9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="W9" t="s">
         <v>49</v>
@@ -1638,7 +1641,7 @@
         <v>53</v>
       </c>
       <c r="V10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="W10" t="s">
         <v>54</v>
@@ -1679,7 +1682,7 @@
         <v>85</v>
       </c>
       <c r="V11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="W11" t="s">
         <v>58</v>
@@ -1714,7 +1717,7 @@
         <v>62</v>
       </c>
       <c r="V12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="W12" t="s">
         <v>63</v>
@@ -1743,7 +1746,7 @@
         <v>67</v>
       </c>
       <c r="V13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="W13" t="s">
         <v>68</v>
@@ -1772,7 +1775,7 @@
         <v>86</v>
       </c>
       <c r="V14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="W14" t="s">
         <v>72</v>
@@ -1798,10 +1801,10 @@
         <v>20</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="W15" t="s">
         <v>45</v>
@@ -1824,10 +1827,10 @@
         <v>3</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="W16" t="s">
         <v>78</v>
@@ -1850,10 +1853,10 @@
         <v>1</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="V17" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="W17" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
added CHESTS chest loot is scriptable in level files changed chest skin added UNLOCK spell looted chests are now saved
</commit_message>
<xml_diff>
--- a/res/items.xlsx
+++ b/res/items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="132" windowWidth="14112" windowHeight="7752"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14115" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="122">
   <si>
     <t>Item ID</t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>-18, -34</t>
+  </si>
+  <si>
+    <t>2, 1</t>
   </si>
 </sst>
 </file>
@@ -1201,13 +1204,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AE8" sqref="AE8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="21" max="21" width="11.44140625" style="1"/>
+    <col min="21" max="21" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -1464,6 +1467,9 @@
       </c>
       <c r="AF5" t="s">
         <v>115</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:33">

</xml_diff>